<commit_message>
adding in main menu
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21160" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21550" uniqueCount="165">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -487,6 +487,30 @@
   </si>
   <si>
     <t xml:space="preserve">Fan2 &lt;&gt; %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temp_pow:&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temp_sound:&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S</t>
   </si>
 </sst>
 </file>
@@ -2310,7 +2334,7 @@
         <v>136</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D22" t="s">
         <v>42</v>
@@ -2424,8 +2448,108 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29"/>
-    <row r="30"/>
+    <row r="29">
+      <c r="B29" t="s">
+        <v>153</v>
+      </c>
+      <c r="C29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="s">
+        <v>155</v>
+      </c>
+      <c r="C30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="s">
+        <v>158</v>
+      </c>
+      <c r="C31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="s">
+        <v>160</v>
+      </c>
+      <c r="C32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>161</v>
+      </c>
+      <c r="C33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" t="s">
+        <v>43</v>
+      </c>
+      <c r="F34" t="s">
+        <v>164</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>